<commit_message>
current work, fixed a data file
removed the “&” sign from the product descriptions, it was causing
formatting problems with the stargazer() table output
</commit_message>
<xml_diff>
--- a/data/Anti-Chafing-Study--master-database.xlsx
+++ b/data/Anti-Chafing-Study--master-database.xlsx
@@ -1525,10 +1525,10 @@
     <t>Gooch Guard Chamois Cream</t>
   </si>
   <si>
-    <t>Zealios All Natural; Vegan; Betwixt Athletic Skin Lubricant &amp; Chamois Cream</t>
-  </si>
-  <si>
-    <t>ChafeZone - Anti-Chafe &amp; Blister Prevention</t>
+    <t>Zealios All Natural; Vegan; Betwixt Athletic Skin Lubricant and Chamois Cream</t>
+  </si>
+  <si>
+    <t>ChafeZone - Anti-Chafe and Blister Prevention</t>
   </si>
   <si>
     <t>http://www.ebay.com/itm/MedZone-ChafeZone-BurnZone-PainZone-LOT-of-20-NEW-First-Aid-Relief-Prevention-/151835007365</t>
@@ -1684,7 +1684,7 @@
     <t>http://www.amazon.com/dp/B001KYVWQG?psc=1</t>
   </si>
   <si>
-    <t>Bag-Balm; Vermonts Original Moisturizing &amp; Softening Ointment</t>
+    <t>Bag-Balm; Vermonts Original Moisturizing and Softening Ointment</t>
   </si>
   <si>
     <t>http://www.amazon.com/Bag-Balm-Vermonts-Original-Moisturizing-Softening/dp/B0014CI4X8</t>
@@ -19504,7 +19504,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="45.29"/>
+    <col customWidth="1" min="2" max="2" width="54.86"/>
     <col customWidth="1" min="3" max="3" width="11.0"/>
     <col customWidth="1" min="4" max="4" width="10.71"/>
     <col customWidth="1" min="5" max="6" width="9.0"/>

</xml_diff>

<commit_message>
fixing a spelling error in a column label
</commit_message>
<xml_diff>
--- a/data/Anti-Chafing-Study--master-database.xlsx
+++ b/data/Anti-Chafing-Study--master-database.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4367" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4367" uniqueCount="838">
   <si>
     <t>Product_ID</t>
   </si>
@@ -1333,10 +1333,10 @@
     <t>Product_Type</t>
   </si>
   <si>
-    <t>Product_Audiance</t>
-  </si>
-  <si>
-    <t>Product_Audiance_Cat2</t>
+    <t>Product_Audience</t>
+  </si>
+  <si>
+    <t>Product_Audience_Cat2</t>
   </si>
   <si>
     <t>Product_Specific_Use</t>
@@ -1351,1123 +1351,1126 @@
     <t>Product_Size_Unit</t>
   </si>
   <si>
+    <t>Product_Unit_Cost_USD</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Rate_5</t>
+  </si>
+  <si>
+    <t>Rate_4</t>
+  </si>
+  <si>
+    <t>Rate_3</t>
+  </si>
+  <si>
+    <t>Rate_2</t>
+  </si>
+  <si>
+    <t>Rate_1</t>
+  </si>
+  <si>
+    <t>Product_Rating_Date</t>
+  </si>
+  <si>
+    <t>Rating_Source</t>
+  </si>
+  <si>
+    <t>Ingredient_Date</t>
+  </si>
+  <si>
+    <t>Ingredient_Source</t>
+  </si>
+  <si>
+    <t>Body Glide Origional</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Amazon.com</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Gold Bond Friction Defense</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Gold-Bond-Friction-Defense-Ounce/dp/B007VC9DKI</t>
+  </si>
+  <si>
+    <t>Skin Stong Slather</t>
+  </si>
+  <si>
+    <t>Cream</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Brave Soldier Friction Zone</t>
+  </si>
+  <si>
+    <t>Ointment</t>
+  </si>
+  <si>
+    <t>Run; Bike</t>
+  </si>
+  <si>
+    <t>Trail Toes Foot and Body Cream</t>
+  </si>
+  <si>
+    <t>Run; Hike</t>
+  </si>
+  <si>
+    <t>Feet</t>
+  </si>
+  <si>
+    <t>HikeGoo Blister Prevention Cream (Feet)</t>
+  </si>
+  <si>
+    <t>Hike</t>
+  </si>
+  <si>
+    <t>rei.com</t>
+  </si>
+  <si>
+    <t>RunGoo Blister Prevention Cream</t>
+  </si>
+  <si>
+    <t>Rocket Pure Friction Therapy Natural Anti-Chafe Balm</t>
+  </si>
+  <si>
+    <t>Triathlon</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Anti-chafe-Protection-Triathletes-Ingredients-Rocket/dp/B00RKHRUFY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaseline </t>
+  </si>
+  <si>
+    <t>Chamois Butt'r</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>Groin</t>
+  </si>
+  <si>
+    <t>BikeBling.com</t>
+  </si>
+  <si>
+    <t>Blue Steel Sports Anti-Chafe Cream</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>Lanacane Anti-Chafing Gel</t>
+  </si>
+  <si>
+    <t>Gel</t>
+  </si>
+  <si>
+    <t>ChafeStop anti-chafing stick</t>
+  </si>
+  <si>
+    <t>2Toms SportShield Liquid Roll-On</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>http://www.2toms.com/products-page/sportshield/sportshield-roll-on/</t>
+  </si>
+  <si>
+    <t>Mission Athletecare 5 Hour Anti-Chafe Cream</t>
+  </si>
+  <si>
+    <t>http://ec2-54-243-178-219.compute-1.amazonaws.com/skindeep/product/525433/MISSION_Athletecare_5_Hour_Anti-Chafe_Cream/</t>
+  </si>
+  <si>
+    <t>Trislide SBR Anti-Chafe Continuous Spray Lubricant</t>
+  </si>
+  <si>
+    <t>http://www.drugstore.com/trislide-aerosol-skin-lubricant/qxp277713</t>
+  </si>
+  <si>
+    <t>SLIK Anti-Friction and Anti-Chafe Skin Lube</t>
+  </si>
+  <si>
+    <t>http://skinstrong.com/slik-anti-chafing-spray/</t>
+  </si>
+  <si>
+    <t>Gooch Guard Chamois Cream</t>
+  </si>
+  <si>
+    <t>Zealios All Natural; Vegan; Betwixt Athletic Skin Lubricant and Chamois Cream</t>
+  </si>
+  <si>
+    <t>ChafeZone - Anti-Chafe and Blister Prevention</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/MedZone-ChafeZone-BurnZone-PainZone-LOT-of-20-NEW-First-Aid-Relief-Prevention-/151835007365</t>
+  </si>
+  <si>
+    <t>Mueller Lube Stick for Runners</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Mueller-Lube-Stick-Runners-2-25-Ounce/dp/B000TS8MHG/ref=pd_sim_sg_16</t>
+  </si>
+  <si>
+    <t>Corona Multi-Purpose Ointment</t>
+  </si>
+  <si>
+    <t>Off-Label</t>
+  </si>
+  <si>
+    <t>Veterinary</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Manna-Pro-0095005392-Purpose-Ointment/dp/B003ARD4TE/ref=sr_1_1?ie=UTF8&amp;qid=1456059201&amp;sr=8-1&amp;keywords=Corona+Multi-Purpose+Ointment</t>
+  </si>
+  <si>
+    <t>Boudreaux's Butt Paste Diaper Rash Ointment Skin Protectant</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Boudreauxs-Butt-Paste-Ointment-Protectant/dp/B001190D5Q/ref=sr_1_4?s=baby-products&amp;ie=UTF8&amp;qid=1456060126&amp;sr=1-4&amp;keywords=Butt+Paste</t>
+  </si>
+  <si>
+    <t>http://www.buttpaste.com/products/original-butt-paste</t>
+  </si>
+  <si>
+    <t>Sportslick</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Sportslick-3-8-oz/dp/B0007OC0A2/ref=sr_1_1?ie=UTF8&amp;qid=1456061443&amp;sr=8-1&amp;keywords=sportslick</t>
+  </si>
+  <si>
+    <t>http://www.allstarhealth.com/de_p/14001/Sportslick_The_Ultimate_Skin_Protector.htm</t>
+  </si>
+  <si>
+    <t>Ruby's Lube - All Natural Anti-Chafe Balm</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Rubys-Lube-Natural-Anti-Chafe-Balm/dp/B00MH7G8GO/ref=sr_1_15?ie=UTF8&amp;qid=1456078186</t>
+  </si>
+  <si>
+    <t>Bodyglide Skin Glide Anti-Friction Balm</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Bodyglide-Skin-Glide-Anti-Friction-Ounce/dp/B0031Y4S0U/ref=sr_1_2?ie=UTF8&amp;qid=1456079038</t>
+  </si>
+  <si>
+    <t>https://www.bodyglide.com/shop/skin/</t>
+  </si>
+  <si>
+    <t>Reflect Sports Hoo Ha Ride Glide</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Reflect-Sports-Ride-Glide-8-Ounce/dp/B009NN2O86</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/forum/-/Tx3RL6DD7J0OV22/ref=ask_dp_dpmw_al_hza?asin=B009NN2O86</t>
+  </si>
+  <si>
+    <t>Aquaphor (Baby)</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Aquaphor-Healing-Ointment-Diaper-Protectant/dp/B001F0RAVQ/ref=sr_1_5?ie=UTF8&amp;qid=1456089783</t>
+  </si>
+  <si>
+    <t>Surf Butta Anti-Chafe Balm</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Surf-Butta-Anti-Chafe-Balm-Eliminates/dp/B017HUPINY/ref=sr_1_9?s=sporting-goods&amp;ie=UTF8&amp;qid=1456090069</t>
+  </si>
+  <si>
+    <t>Chamois Butt'r GoStik Skin Lubricant</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Chamois-Buttr-GoStik-Lubricant-2-5-Ounce/dp/B00M8YXR74/ref=sr_1_18?s=sporting-goods&amp;ie=UTF8&amp;qid=1456090069</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Chamois-Buttr-GoStik-Lubricant-2-5-Ounce/dp/B00M8YXR74%3FSubscriptionId%3DAKIAJ7ULU7QZXKP7GIOQ%26tag%3Dhomea0c-20%26linkCode%3Dxm2%26camp%3D2025%26creative%3D165953%26creativeASIN%3DB00M8YXR74</t>
+  </si>
+  <si>
+    <t>Dead Down Wind Anti-Chafe + Anti-Itch Lotion</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Dead-Down-Wind-Anti-Chafe-Anti-Itch/dp/B00OH5LVLQ/ref=sr_1_1?ie=UTF8&amp;qid=1456091893</t>
+  </si>
+  <si>
+    <t>That Butt Stuff Anti Chafing Cream - Natural Chamois Balm</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Anti-Chafing-Cream-Natural-Chamois/dp/B002TIIGIO/ref=sr_1_31?s=sporting-goods&amp;ie=UTF8&amp;qid=1456107746</t>
+  </si>
+  <si>
+    <t>Petal Power Joy Ride Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/dp/B00PM94YC4?psc=1 PRICE information from manufactor website http://www.petal-power.com/store/p2/Petal_Power_Joy_Ride_Creme.html</t>
+  </si>
+  <si>
+    <t>http://www.petal-power.com/our-ingredients.html</t>
+  </si>
+  <si>
+    <t>DZ Nuts Pro Chamois Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/DZ-Nuts-Pro-Chamois-Cream/dp/B008F9J16M/ref=pd_sbs_468_5?ie=UTF8&amp;dpID=31ai7kgn6oL&amp;dpSrc=sims&amp;preST=_AC_UL160_SR160%2C160_&amp;refRID=1RF8866Y6MXDJFBDEJ84</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/forum/-/Tx4H8S2UKHM9D2/-/ref=ask_dp_lsw_al_hza?asin=B001C6DIF0  http://www.competitivecyclist.com/dz-nuts-pro-chamios-cream-mens</t>
+  </si>
+  <si>
+    <t>Soigneur Chamois Cream - Tempo</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Soigneur-Tempo-Chamois-Cream/dp/B009FPGHN0/ref=sr_1_1?ie=UTF8&amp;qid=1456200002</t>
+  </si>
+  <si>
+    <t>http://www.soigneur.net/shop/chamois-cream-1</t>
+  </si>
+  <si>
+    <t>Beach Gladiator Anti-Chafe Roll-On Rash Guard for Beach/Surf Rash</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Beach-Gladiator-Anti-Chafe-Roll--Guard/dp/B00RPOQMEC</t>
+  </si>
+  <si>
+    <t>Monistat Soothing Care Chafing Relief Powder-Gel</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Monistat-Soothing-Chafing-Powder-Gel-1-5-Ounce/dp/B0012ZNSWE</t>
+  </si>
+  <si>
+    <t>Assos Chamois Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Assos-Chamois-Cream-4-73-oz/dp/B001O19E2E</t>
+  </si>
+  <si>
+    <t>Udderly Smooth Chamois Cream with Shea Butter</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Udderly-Smooth-Chamois-Cream-Butter/dp/B00D86VJD0</t>
+  </si>
+  <si>
+    <t>Moraz Redskin - Polygonum Anti Chafe Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/dp/B001KYVWQG?psc=1</t>
+  </si>
+  <si>
+    <t>Bag-Balm; Vermonts Original Moisturizing and Softening Ointment</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Bag-Balm-Vermonts-Original-Moisturizing-Softening/dp/B0014CI4X8</t>
+  </si>
+  <si>
+    <t>Doc's Skin Care Chamois Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Docs-Skin-Care-Chamois-Cream/dp/B00EOUTNPA</t>
+  </si>
+  <si>
+    <t>http://docsskincare.com/products/chamois-cream/</t>
+  </si>
+  <si>
+    <t>Hammer Nutrition Seat Saver Chamois And Anti- Chafing Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Hammer-Nutrition-Saver-Chamois-Chafing/dp/B002K69HSI/</t>
+  </si>
+  <si>
+    <t>http://www.hammernutrition.com/products/seat-saver.ssv.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RunGuard Anti-Chafe Stick </t>
+  </si>
+  <si>
+    <t>https://www.google.com/shopping/product/4682990999738067527?q=RunGuard+Anti-Chafe&amp;biw=1192&amp;bih=578&amp;bav=on.2;or.r_cp.&amp;bvm=bv.115339255;d.dmo&amp;tch=1&amp;ech=1&amp;psi=pSzRVtiUAcHxeq6olYgH.1456549138121.9&amp;prds=hsec:reviews;paur:ClkAsKraX_JVZz_TOWlQw69jyl1NsFlF2fJED_TB-hXY0Ys4Ufb3VKbRAncj0n_e6kKDkYTBLlJNxS4V-4lKNaAn68oW1iNyTRR0HzndpgfJRZ2Ppr8O50f6xxIZAFPVH70i1tOHBnSoJG3SX9zlZEkaNSfmTQ&amp;ved=0ahUKEwjivqvilJfLAhVHGB4KHX1fB_AQqisIFQ&amp;ei=fC3RVuKQBseweP2-nYAP</t>
+  </si>
+  <si>
+    <t>http://www.runguards.com/products/runguard-original/ingredients</t>
+  </si>
+  <si>
+    <t>Fresh Balls</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Fresh-Balls-Oz-Tube-Pack/dp/B00D3LTEVE/#customerReviews</t>
+  </si>
+  <si>
+    <t>Akileïne Sports NOK Anti-chafing Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Akile%C3%AFne-Sports-Anti-chafing-Cream-75ml/dp/B0070X231Y; http://www.mec.ca/product/5009-478/sports-akileine-anti-friction-nok-cream-75ml/</t>
+  </si>
+  <si>
+    <t>http://www.cocooncenter.co.uk/akileine-sports-nok-anti-chafing-cream-75ml/8534.html#composition</t>
+  </si>
+  <si>
+    <t>Shea Butter Market SPLAX Anti‑Chafing Stick</t>
+  </si>
+  <si>
+    <t>http://www.mec.ca/product/5014-984/shea-butter-market-splax-anti-chafing-stick-60g/</t>
+  </si>
+  <si>
+    <t>http://www.artisancraftedbodycare.com/shea-butter-market-splax-anti-chafing-stick</t>
+  </si>
+  <si>
+    <t>Miracle of Aloe Chafe Guard Anti Friction Stick</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Miracle-Aloe-Lubricants-Eliminates-Comfortable/dp/B002FPBPOI</t>
+  </si>
+  <si>
+    <t>http://www.miracleofaloe.com/personal-care/problem-solvers/chafe-guard.html</t>
+  </si>
+  <si>
+    <t>Uberlube Luxury Lubricant</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Uberlube-UBER-100-Luxury-Lubricant-100ml/dp/B00502KJ2C</t>
+  </si>
+  <si>
+    <t>GurneyGoo Lubricant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General </t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/GurneyGears-GurneyGoo-Anti-Chafe-85ml/dp/B00SQ1DQY2</t>
+  </si>
+  <si>
+    <t>Desitin Maximum Strength Paste</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/dp/B003O32P8U/</t>
+  </si>
+  <si>
+    <t>https://www.desitin.com/diaper-rash-products/maximum-strength-original-zinc-oxide-paste</t>
+  </si>
+  <si>
+    <t>Hipoglos 4.2 Oz Baby Diaper Rash Cream And Skin Protectant</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Hipoglos-Baby-Diaper-Cream-Protectant/dp/B004DAQWAK</t>
+  </si>
+  <si>
+    <t>http://dailymed.nlm.nih.gov/dailymed/archives/fdaDrugInfo.cfm?archiveid=42792</t>
+  </si>
+  <si>
+    <t>Cramer Skin Lube</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Cramer-Legendary-Lubricant-Marathons-Triathlons/dp/B0002V8R70</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/NEW-Cramer-Skin-Lube-Pro-Strength-Lubricating-Ointment-1-Lb-Tub-192538-Chafing-/181714844162?hash=item2a4f0c7a02:g:lOMAAOSwNSxVKdu5</t>
+  </si>
+  <si>
+    <t>Waxelene Petroleum Jelly Alternative</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Waxelene-Petroleum-Jelly-Alternative-9-Ounce/dp/B00D3PMP20/</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/forum/-/Tx2LNYLMMZS5CUQ/-/ref=ask_dp_lsw_al_hza?asin=B00D3PMP20</t>
+  </si>
+  <si>
+    <t>Band-Aid Friction Blister Block Stick</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Band-Aid-Friction-Blister-Block-Stick/dp/B00166FZBG/</t>
+  </si>
+  <si>
+    <t>ChafeX Anti-Chafing Skin Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/gp/product/B00TT3KRMK/</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/forum/-/Tx2QO7ANIQVQO8C/ref=ask_dp_dpmw_al_hza?asin=B00TT3KRMK</t>
+  </si>
+  <si>
+    <t>Neat Feat 3B Body Saver Skin Chafing Antiperspirant Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Neat-Saver-Chafing-Antiperspirant-Ounces/dp/B00B5MPCWI</t>
+  </si>
+  <si>
+    <t>Neat 3B Action Cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.co.uk/dp/B001D8D7D0</t>
+  </si>
+  <si>
+    <t>3M Cavilon Durable Barrier Cream Fragrance Free</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/3M-Cavilon-Durable-Barrier-Fragrance/dp/B00CYPUUYK</t>
+  </si>
+  <si>
+    <t>http://solutions.3m.co.uk/wps/portal/3M/en_GB/Cavilon/skin-care/products/durable-barrier-cream/</t>
+  </si>
+  <si>
+    <t>Avon basics silicone glove hand cream</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/basics-silicone-glove-cream-3-4fl/dp/B0014HG8W2/</t>
+  </si>
+  <si>
+    <t>https://www.avon.com/product/41894/avon-care-silicone-glove-protective-hand-cream?setlang=en</t>
+  </si>
+  <si>
+    <t>Ingredient_Alternate_Name</t>
+  </si>
+  <si>
+    <t>Ingredient_Definition</t>
+  </si>
+  <si>
+    <t>Ingredient_Definition_Source</t>
+  </si>
+  <si>
+    <t>Ingredient_Def_Date</t>
+  </si>
+  <si>
+    <t>Ingredient_Chem_Ref</t>
+  </si>
+  <si>
+    <t>8-HYDROXYQUINOLINE</t>
+  </si>
+  <si>
+    <t>8-HYDROXYQUINOLINE is an antiseptic with mild fungistatic; bacteriostatic; anthelmintic; and amebicidal action. It is also used as a reagent and metal chelator; as a carrier for radio-indium for diagnostic purposes; and its halogenated derivatives are used in addition as topical anti-infective agents and oral antiamebics.</t>
+  </si>
+  <si>
+    <t>https://pubchem.ncbi.nlm.nih.gov/compound/8-hydroxyquinoline#section=Top</t>
+  </si>
+  <si>
+    <t>ACACIA DECURRENS Extract</t>
+  </si>
+  <si>
+    <t>About ACACIA DECURRENS FLOWER WAX: Acacia Decurrens Flower Wax is a wax obtained from the flowers of Acacia decurrens. Function(s): Skin-Conditioning Agent - Emollient; Skin-Conditioning Agent - Occlusive; SKIN CONDITIONING; SKIN PROTECTING</t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient/716261/ACACIA_DECURRENS_FLOWER_WAX/</t>
+  </si>
+  <si>
+    <t>Acai Juice</t>
+  </si>
+  <si>
+    <t>PH Control. Acetic Acid is an organic acid formed when ethanol is fermented. Vinegar is typically a 5% solution of Acetic Acid. Brown Rice Vinegar is the vinegar produced by the fermentation of unpolished brown rice. Natural Vinegars also contain small amounts of tartaric acid; citric acid and other acids. In cosmetics and personal care products; Acetic Acid; Vinegar and Brown Rice Vinegar are used in the formulation of hair conditioners; shampoos; hair rinses; wave sets and other hair care products. Acetic Acid is also used in mouthwashes and breath fresheners and Vinegar can be found in skin care products.</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/vinegar-and-acetic-acid</t>
+  </si>
+  <si>
+    <t>Acrylate Polymer</t>
+  </si>
+  <si>
+    <t>Binding agent. Acrylate polymer; "three" or "ter" in terpolymer means three monomers connected together.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Acrylate_polymer</t>
+  </si>
+  <si>
+    <t>Detatured Alcohol? Ethanol?</t>
+  </si>
+  <si>
+    <t>Unclear to which "alcohol" this is.</t>
+  </si>
+  <si>
+    <t>5-Ureidohydantoin; Glyoxyldiureide</t>
+  </si>
+  <si>
+    <t>llantoin is a naturally ocurring nitrogenous compound used as a skin conditioning agent.</t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient/700244/ALLANTOIN/</t>
+  </si>
+  <si>
+    <t>https://fscimage.fishersci.com/msds/24578.htm</t>
+  </si>
+  <si>
+    <t>Aloe Vera Extract; Aloe Vera Juice; Aloe Leaf Juice; Aloe Vera Gel</t>
+  </si>
+  <si>
+    <t>Juice vs. Gel -- Gel has a higher polysachride content; made from the inside of the plant. Juice is made from the outer leaf mainly. Gel has a higher concentration of aloin; which is a laxitive (why you should not drink the gel!)</t>
+  </si>
+  <si>
+    <t>http://www.livestrong.com/article/474409-aloe-vera-gel-vs-juice/ ; http://www.lilyofthedesert.com/faq/</t>
+  </si>
+  <si>
+    <t>Nutrients are transfered from the plant by mixing the gel with oil and sperating it out</t>
+  </si>
+  <si>
+    <t>http://www.aloeplant.info/how-to-make-aloe-vera-oil-for-skin/</t>
+  </si>
+  <si>
+    <t>ALUMINUM HYDROXYCHLORIDE</t>
+  </si>
+  <si>
+    <t>Aluminium chlorohydrate is a group of specific aluminium salts having the general formula AlnCl(3n-m)(OH)m. It is used in deodorants and antiperspirants and as a coagulant in water purification.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Aluminium_chlorohydrate</t>
+  </si>
+  <si>
+    <t>ALUMINUM SALT STARCH</t>
+  </si>
+  <si>
+    <t>This ingredient is an aluminum salt of chemically modified starch. Function(s): Absorbent; Anticaking Agent; Viscosity Increasing Agent - Nonaqueous; VISCOSITY CONTROLLING</t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient/700326/ALUMINUM_STARCH_OCTENYLSUCCINATE/</t>
+  </si>
+  <si>
+    <t>Prunus Armeniaca (Apricot) Oil; Bitter Almond Oil</t>
+  </si>
+  <si>
+    <t>Prunus Armeniaca (Apricot) Kernel Oil and Hydrogenated Apricot Oil function as skin conditioning agents - occlusive. Hydrogenated Apricot Kernel Oil also functions as a viscosity increasing agents - nonaqueous.</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/prunus-armeniaca-apricot-kernel-oil-and-hydrogenated-apricot-kernel-oil</t>
+  </si>
+  <si>
+    <t>ASCORBYL PALMITATE (VITAMIN C PALMITATE)</t>
+  </si>
+  <si>
+    <t>Ascorbyl palmitate is an ester formed from ascorbic acid and palmitic acid creating a fat-soluble form of vitamin C. In addition to its use as a source of vitamin C; it is also used as an antioxidant food additive (E number E304).</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Ascorbyl_palmitate</t>
+  </si>
+  <si>
+    <t>White Beeswax; Yellow Beeswax</t>
+  </si>
+  <si>
+    <t>Desyl Alcohol; Bitter Almond Oil Camphor</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Benzoin</t>
+  </si>
+  <si>
+    <t>BENZENEMETHANOL; BENZYLIC ALCOHOL; PHENYLCARBINOL; PHENYLMETHANOL; PHENYLMETHYL ALCOHOL;</t>
+  </si>
+  <si>
+    <t>External Analgesic; Fragrance Ingredient; Oral Health Care Drug; Preservative; Solvent;Viscosity Decreasing Agent; MASKING</t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient/700697/BENZYL_ALCOHOL/</t>
+  </si>
+  <si>
+    <t>http://chem.sis.nlm.nih.gov/chemidplus/name/benzyl%20alcohol</t>
+  </si>
+  <si>
+    <t>Beta-Carotene is a naturally occurring carotenoid pigment found in many fruits and vegetables. Beta-Carotene is a precursor of; and can be synthesized from; vitamin A. Beta-Carotene used in cosmetics and personal care products is prepared synthetically or obtained from natural sources.</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/beta-carotene</t>
+  </si>
+  <si>
+    <t>Butylated hydroxyanisole is an antioxidant consisting of a mixture of two isomeric organic compounds; 2-tert-butyl-4-hydroxyanisole and 3-tert-butyl-4-hydroxyanisole. It is prepared from 4-methoxyphenol and isobutylene</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Butylated_hydroxyanisole</t>
+  </si>
+  <si>
+    <t>Chamomile; Chamomile Extract</t>
+  </si>
+  <si>
+    <t>A resin obtained from Chamomile. Reduces sensitivity and inflammation.</t>
+  </si>
+  <si>
+    <t>https://www.dermalinstitute.com/us/library/glossary.html?l=B</t>
+  </si>
+  <si>
+    <t>Propellent</t>
+  </si>
+  <si>
+    <t>Butane is a gas commenly used as a propellent in aerosal sprays</t>
+  </si>
+  <si>
+    <t>Calendula officinalis Extract; Pot Marigold; Calendula Flower Extract; Calendula Flower Oil</t>
+  </si>
+  <si>
+    <t>In cosmetics and personal care products; Calendula Officinalis Extract; Calendula Officinalis Flower Extract and Calendula Officinalis Flower Oil function as skin conditioning agents - miscellaneous. Calendula Officinalis Flower Extract and Calendula Officinalis Flower Oil also function as fragrance ingredients. Calendula Officinalis Seed Oil functions as a skin conditioning agent - occlusive.</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/calendula-officinalis-derived-ingredients</t>
+  </si>
+  <si>
+    <t>These waxes also increase the thickness of the lipid (oil) portion of solid and stick-like products such as lipstick; giving them structure; allowing for a smooth application; and keeping them solid. Candelilla Wax is a yellowish-brown hard; brittle lustrous solid; extracted from the surface of the plant Euphorbia cerifera. In Europe this wax is known as Candelilla Cera.</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/beeswax-and-plant-waxes</t>
+  </si>
+  <si>
+    <t>Caprylic/Capric Triglycerides. * A mixed triester derived from coconut oil and glycerin. It comes in the form of an oily liquid; and is sometimes mistakenly referred to as fractionated coconut oil. Functions: Caprylic mainly works as an emollient; dispersing agent and solvent.</t>
+  </si>
+  <si>
+    <t>https://www.truthinaging.com/ingredients/capryliccapric-triglycerides</t>
+  </si>
+  <si>
+    <t>Properties: Effective humectant and emollient with antimicrobial efficacy; boosts traditional preservatives; provides deodorizing efficacy.</t>
+  </si>
+  <si>
+    <t>http://www.makingcosmetics.com/Caprylyl-Glycol-EHG_p_159.html</t>
+  </si>
+  <si>
+    <t>Castor Seed Oil; Ricinus Cummunis (Castor Seed) Oil</t>
+  </si>
+  <si>
+    <t>Ceresin wax</t>
+  </si>
+  <si>
+    <t>Cerin; Cerasin; Cerosin; Ceresin Wax; Ceresine</t>
+  </si>
+  <si>
+    <t>is a wax derived from ozokerite by a purifying process.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Ceresin</t>
+  </si>
+  <si>
+    <t>Cetearyl Alcohol and the other fatty alcohols keep an emulsion from separating into its oil and liquid components. These ingredients are also used to alter the thickness of liquid products and to increase foaming capacity or to stabilize foams.</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/cetearyl-alcohol-and-related-ingredients</t>
+  </si>
+  <si>
+    <t>Cetyl Esters NF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cetyl Esters Wax offers an easy way to increase the viscosity (thickness) of your creams and lotions while also improving the feel.  There is some confusion about the naturalness of this material because it is referred to as a synthetic Spermaceti Wax.  Spermaceti Wax is waxy liquid harvested from Whales; and when the industry realized that there was a demand for a more friendly approach they created the synthetic alternative; Cetyl Esters Wax; which is natural wax produced from coconut.  </t>
+  </si>
+  <si>
+    <t>http://www.ingredientstodiefor.com/item/Cetyl_Esters_NF/142/</t>
+  </si>
+  <si>
+    <t>Phenylacrylic acid</t>
+  </si>
+  <si>
+    <t>Cinnamic acid is an organic compound with the formula C6H5CHCHCO2H. It is a white crystalline compound that is slightly soluble in water; and freely soluble in many organic solvents. Classified as an unsaturated carboxylic acid; it occurs naturally in a number of plants.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Cinnamic_acid</t>
+  </si>
+  <si>
+    <t>Cocoa Seed Butter; Theobroma Cacao (Cocoa Seed) Butter</t>
+  </si>
+  <si>
+    <t>Comfrey; Comfrey Root Extract</t>
+  </si>
+  <si>
+    <t>CYCLOPENTASILOXANE</t>
+  </si>
+  <si>
+    <t>ANTISTATIC; EMOLLIENT; HAIR CONDITIONING; HUMECTANT; SOLVENT; VISCOSITY CONTROLLING</t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient/701738/CYCLOMETHICONE/</t>
+  </si>
+  <si>
+    <t>http://chem.sis.nlm.nih.gov/chemidplus/rn/69430-24-6</t>
+  </si>
+  <si>
+    <t>CYCLOPENTASILOXANE; DECAMETHYL-; DECAMETHYL- CYCLOPENTASILOXANE; DECAMETHYLCYCLOPENTASILOXANE</t>
+  </si>
+  <si>
+    <t>Decamethylcyclopentasiloxane is an organosilicon compound with the formula [(CH₃)₂SiO]₅. It is a colorless and odorless liquid that is slightly volatile. The compound is classified as a cyclomethicone.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Decamethylcyclopentasiloxane</t>
+  </si>
+  <si>
+    <t>https://pubchem.ncbi.nlm.nih.gov/compound/decamethylcyclopentasiloxane#section=Top</t>
+  </si>
+  <si>
+    <t>Methanol; Methyl Alcohol; Wood Alcohol</t>
+  </si>
+  <si>
+    <t>Diazolidnyl Urea</t>
+  </si>
+  <si>
+    <t>Diazolidinylurea</t>
+  </si>
+  <si>
+    <t>Diazolidinyl urea is an antimicrobial preservative used in cosmetics. It is chemically related to imidazolidinyl urea which is used in the same way. Diazolidinyl urea acts as a formaldehyde releaser.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Diazolidinyl_urea</t>
+  </si>
+  <si>
+    <t>http://www.commonchemistry.org/ChemicalDetail.aspx?ref=78491-02-8</t>
+  </si>
+  <si>
+    <t>Polydimethylsiloxane; Octamethyltrisiloxane; Dimethicone Crosspolymer</t>
+  </si>
+  <si>
+    <t>Polydimethylsiloxane belongs to a group of polymeric organosilicon compounds that are commonly referred to as silicones. PDMS is the most widely used silicon-based organic polymer; and is particularly known for its unusual rheological properties.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Polydimethylsiloxane</t>
+  </si>
+  <si>
+    <t>https://pubchem.ncbi.nlm.nih.gov/compound/24705</t>
+  </si>
+  <si>
+    <t>Ethylenediamine Tetraacetic Acid; Tetrasodium EDTA; Disodium EDTA</t>
+  </si>
+  <si>
+    <t>Disodium EDTA and the related ingredients bind to metal ions which inactivates them. The binding of metal ions helps prevent the deterioration of cosmetics and personal care products. It also helps to maintain clarity; protect fragrance compounds; and prevent rancidity.</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/edta-and-related-ingredients</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/ozokerite-and-other-fossil-and-synthetic-waxes</t>
+  </si>
+  <si>
+    <t>Ethylhexyglycerine</t>
+  </si>
+  <si>
+    <t>glycerine; propanetriol; 1;2;3-trihydroxypropane</t>
+  </si>
+  <si>
+    <t>Glycerol is a simple polyol (sugar alcohol) compound. It is a colorless; odorless; viscous liquid that is widely used in pharmaceutical formulations.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Glycerol</t>
+  </si>
+  <si>
+    <t>Glyceryl behenate is a fat used in cosmetics; foods; and oral pharmaceutical formulations. In cosmetics; it is mainly used as a viscosity-increasing agent in emulsions. Wikipedia</t>
+  </si>
+  <si>
+    <t>http://en.wikipedia.org/wiki/Glyceryl_behenate</t>
+  </si>
+  <si>
+    <t>https://pubchem.ncbi.nlm.nih.gov/compound/Glyceryl_behenate</t>
+  </si>
+  <si>
+    <t>Glycerin Stearate; Glycerol Monostearate</t>
+  </si>
+  <si>
+    <t>A humectant from the nectar of flowers.</t>
+  </si>
+  <si>
+    <t>https://www.dermalinstitute.com/us/library/glossary.html?l=H</t>
+  </si>
+  <si>
+    <t>Synthetic avenanthramide (Oat active)</t>
+  </si>
+  <si>
+    <t>Synthetic avenanthramide (Oat active) used to boost the efficacy of natural Oat.</t>
+  </si>
+  <si>
+    <t>Wax</t>
+  </si>
+  <si>
+    <t>Linalool is a naturally occurring fragrance substance produced by a wide variety of plants such as mint; cinnamon; citrus fruits; and birch trees. Linalool can also be produced synthetically.</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/linalool</t>
+  </si>
+  <si>
+    <t>Menthyl Lactate is a solid cooling agent and fragrance component for cosmetics. It is a derivative of Menthol; but is milder and more compatible with the skin.</t>
+  </si>
+  <si>
+    <t>http://www.makingcosmetics.com/Menthyl-Lactate_p_676.html</t>
+  </si>
+  <si>
+    <t>checkerberry oil; gaultheria oil; sweet birch oil; wintergreen oil</t>
+  </si>
+  <si>
+    <t>The methyl ester of salicylic acid; produced synthetically or distilled from Gaultheria procumbens (family Ericaceae) or from Betula lenta (family Betulaceae); used externally and internally for the treatment of various forms of rheumatism.</t>
+  </si>
+  <si>
+    <t>http://www.drugs.com/dict/methyl-salicylate.html</t>
+  </si>
+  <si>
+    <t>http://chem.sis.nlm.nih.gov/chemidplus/rn/119-36-8</t>
+  </si>
+  <si>
+    <t>Methylparaben is an anti-fungal agent often used in a variety of cosmetics and personal-care products. It is also used as a food preservative and has the E number E218.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Methylparaben</t>
+  </si>
+  <si>
+    <t>Paraffinum Liquidum; White Mineral Oil (Paraffinum Liquidum)</t>
+  </si>
+  <si>
+    <t>Octyldocecanol</t>
+  </si>
+  <si>
+    <t>Europaea (Olive) Fruit Unsaponifiables is a fraction of olive fruit remaining after fractional distillation.</t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient/721077/OLEA_EUROPAEA_%28OLIVE%29_FRUIT_UNSAPONIFIABLES/</t>
+  </si>
+  <si>
+    <t>Panthenol (pantothenol) is the alcohol analog of pantothenic acid (vitamin B5); and is thus a provitamin of B5. In organisms it is quickly oxidized to pantothenate [pantothenic acid]. In cosmetics and personal-care products; panthenol is a humectant; emollient; and moisturizer. In ointments; panthenol is an effective skin penetrator.[2] It is sometimes mixed with allantoin; in concentrations of up to 2-5%; and is used for treatment of sunburns; mild burns and minor skin disorders.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Panthenol</t>
+  </si>
+  <si>
+    <t>Myroxylon pereirae; Peruvian balsam; Indian balsam; black balsam; balsam Peru</t>
+  </si>
+  <si>
+    <t>Peru balsam is a tall tree that grows in Central America. This large tree often is cultivated as a shade tree. Crude Peru balsam is a dark brown; thick liquid with an aromatic smell of cinnamon and vanilla; and bitter taste. To remove it from the tree; the bark is alternately scorched and beaten.</t>
+  </si>
+  <si>
+    <t>http://www.drugs.com/npc/peru-balsam.html</t>
+  </si>
+  <si>
+    <t>Amur cork tree</t>
+  </si>
+  <si>
+    <t>Phellodendron amurense Rupr. is a species of tree in the family Rutaceae; commonly called the Amur cork tree. It is a major source of huáng bò (Chinese: 黄柏 or 黄檗); one of the 50 fundamental herbs used in traditional Chinese medicine. The Ainu people used this plant; called shikerebe-ni; as a painkiller</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Phellodendron_amurense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenoxyethanol is an oily; slightly sticky liquid with a faint rose-like scent. It is used as a preservative in a wide variety of cosmetic and personal care products; including skin care products; eye makeup; fragrances; blushers; foundations; lipstick; bath soaps and detergents; etc. Research shows that this ingredient is safe when used in these products. </t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/phenoxyethanol</t>
+  </si>
+  <si>
+    <t>Polyphenylmethyl siloxane</t>
+  </si>
+  <si>
+    <t>Phenyl Trimethicone is a derivative of silica; or silcione; and is used in cosmetics and beauty products as an anti-foaming agent; hair conditioning agent; and skin-conditioning agent (Cosmetic Database)</t>
+  </si>
+  <si>
+    <t>https://www.truthinaging.com/ingredients/phenyl-trimethicone</t>
+  </si>
+  <si>
+    <t>https://pubchem.ncbi.nlm.nih.gov/compound/Phenyltris_trimethylsiloxy_silane#section=Top</t>
+  </si>
+  <si>
+    <t>Polygonum Aviculare</t>
+  </si>
+  <si>
+    <t>knotgrass; knotweed; pigweed</t>
+  </si>
+  <si>
+    <t>Polygonum aviculare or common knotgrass is a plant related to buckwheat and dock. It is also calledprostrate knotweed; birdweed; pigweed and lowgrass. It is an annual found in fields and wasteland; with white flowers from June to October. It is widespread across many countries in temperate regions; apparently native to Eurasia and North America; naturalized in temperate parts of the Southern Hemisphere.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Polygonum_aviculare</t>
+  </si>
+  <si>
+    <t>Gas used as a propellent in aerosol sprays</t>
+  </si>
+  <si>
+    <t>Propylene glycol; α-Propylene glycol; 1;2-Propanediol; 1;2-Dihydroxypropane; Methyl ethyl glycol (MEG); Methylethylene glycol</t>
+  </si>
+  <si>
+    <t>Propylene glycol; also called propane-1;2-diol; is an organic compound with the chemical formula C₃H₈O₂. It is a viscous colourless liquid which is nearly odourless but possesses a faintly sweet taste.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Propylene_glycol</t>
+  </si>
+  <si>
+    <t>Rosemary Leaf Extract; Rosmarinus Officinalis (Rosemary) Leaf Extract</t>
+  </si>
+  <si>
+    <t>beta hydroxy acid (abbreviated BHA);2-Hydroxybenzoic acid</t>
+  </si>
+  <si>
+    <t>Antiacne Agent; Antidandruff Agent; Corn/Callus/Wart Remover; Denaturant; Exfoliant;Fragrance Ingredient; Hair Conditioning Agent; Skin-Conditioning Agent - Miscellaneous; KERATOLYTIC; MASKING; PRESERVATIVE; SKIN CONDITIONING</t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient/705746/SALICYLIC_ACID/</t>
+  </si>
+  <si>
+    <t>http://chem.sis.nlm.nih.gov/chemidplus/name/salicylic%20acid</t>
+  </si>
+  <si>
+    <t>Silicone</t>
+  </si>
+  <si>
+    <t>2;4-hexadienoic acid</t>
+  </si>
+  <si>
+    <t>Sorbic acid (C6H8O2) is a natural preservative that comes from the rowan berries; Sorbus aucuparia (family Rosaceae). It is also prepared synthetically. It inhibits growth of fungi; yeast; mold and some bacteria and is nearly nontoxic to humans. Sorbic acid is safe to use in a wide range of foods; drugs; and cosmetic products. Sorbic acid and its salts; sodium sorbate; potassium sorbate and calcium sorbate are often used in food products as preservatives.</t>
+  </si>
+  <si>
+    <t>http://www.drugs.com/inactive/sorbic-acid-81.html</t>
+  </si>
+  <si>
+    <t>https://pubchem.ncbi.nlm.nih.gov/compound/643460</t>
+  </si>
+  <si>
+    <t>Soy Oil</t>
+  </si>
+  <si>
+    <t>Dimethicone; also known as polydimethylsiloxane; is a silicon-based polymer that is a man-made synthetic molecule made up of repeating units called monomers.  Silicon is the second most abundant element in the Earth's crust after oxygen; and silicon dioxide is also known as sand; commonly found on beaches and shores.  Dimethicone can also be found in many cooking oils; processed foods and in fast food items such as chicken nuggets and French fries</t>
+  </si>
+  <si>
+    <t>http://www.cosmeticsinfo.org/ingredient/stearyl-dimethicone</t>
+  </si>
+  <si>
+    <t>http://chem.sis.nlm.nih.gov/chemidplus/name/startswith/stearyl%20dimethicone</t>
+  </si>
+  <si>
+    <t>Steric Acid</t>
+  </si>
+  <si>
+    <t>Melaleuca Alternifolia (Tea Tree) Extract or Leaf Oil</t>
+  </si>
+  <si>
+    <t>Used for its antiseptic; analgesic and anti-bacterial properties; also aids in healing and soothing the skin.</t>
+  </si>
+  <si>
+    <t>https://www.dermalinstitute.com/us/library/glossary.html?l=M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triethanolamine is a strongly alkaline substance used as surfactant and pH adjusting chemical. Function(s): Fragrance Ingredient; pH Adjuster; Surfactant - Emulsifying Agent; BUFFERING; </t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient.php?ingred06=706639</t>
+  </si>
+  <si>
+    <t>OCTAMETHYL- TRISILOXANE; OCTAMETHYLTRISILOXANE; OCTAMETHYLTRISILOXANE; OCTAMETHYLTRISILOXANE; TRISILOXANE; OCTAMETHYL; TRISILOXANE; OCTAMETHYL-</t>
+  </si>
+  <si>
+    <t>About TRISILOXANE: Trisiloxane is a linear siloxane. Function(s): Antifoaming Agent; Skin-Conditioning Agent - Miscellaneous; SKIN CONDITIONING</t>
+  </si>
+  <si>
+    <t>http://www.ewg.org/skindeep/ingredient/706714/TRISILOXANE/</t>
+  </si>
+  <si>
+    <t>https://pubchem.ncbi.nlm.nih.gov/compound/vanillin#section=Top</t>
+  </si>
+  <si>
+    <t>Tocopheryl; Tocopherols; Tocopheryl Acetate Vitamin E Acetate; DL Alpha Tocopherol; Mixed Tocopherols</t>
+  </si>
+  <si>
+    <t>Tocopheryl acetate; also known as vitamin E acetate; is a common vitamin supplement with the molecular formula C31H52O3 (for 'α' form). It is the ester of acetic acid and tocopherol (vitamin E). It is often used indermatological products such as skin creams. Tocopheryl acetate is not oxidized and can penetrate through the skin to the living cells; where about 5% is converted to free tocopherol and provides beneficial antioxidant effects.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Tocopheryl_acetate</t>
+  </si>
+  <si>
+    <t>Aqua; Deionized Water</t>
+  </si>
+  <si>
+    <t>Epilobium Angustifolium; Willow Herb; Willow Herb Flower/Leaf/Stem Extract</t>
+  </si>
+  <si>
+    <t>Epilobium angustifolium is a PERENNIAL growing to 2 m (6ft) by 1 m (3ft 3in) at a fast rate.</t>
+  </si>
+  <si>
+    <t>http://www.pfaf.org/user/plant.aspx?LatinName=Epilobium+angustifolium</t>
+  </si>
+  <si>
+    <t>Achillea Millefolium</t>
+  </si>
+  <si>
+    <t>Achillea millefolium; commonly known as yarrow /ˈjæroʊ/ or common yarrow; is a flowering plant in the family Asteraceae. It is native to temperate regions of the Northern Hemisphere in Asia; Europe; and North America.[1] It has been introduced as a feed for live stock in places like New Zealand[2] and Australia. However; it is a weed in those places[2] and sometimes also in its native regions.[3]</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Achillea_millefolium</t>
+  </si>
+  <si>
+    <t>Zinc Oxide (CI 77947)</t>
+  </si>
+  <si>
+    <t>Zinc Stearate</t>
+  </si>
+  <si>
+    <t>General Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are no "blank" values; where no data was entered; the value of "na" was assigned. </t>
+  </si>
+  <si>
+    <t>Ingredients.csv: Assigns Ingredients to Products</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Index value for anti-chafe products from the Product_Rating table</t>
+  </si>
+  <si>
+    <t>Index value for anti-chafe ingredient from the Ingredient Defs (Definitions) table</t>
+  </si>
+  <si>
+    <t>Standardized ingredient name. Many products use different or alternate names. This provides some commonality.</t>
+  </si>
+  <si>
+    <t>Order of the ingredient from the product label. In theory; the first ingredient is the largest component; and listed in decending order</t>
+  </si>
+  <si>
+    <t>If a substitution was made for the common name; the original label ingredient listed is preserved here</t>
+  </si>
+  <si>
+    <t>Any minor notes about an ingredient for informational purposes</t>
+  </si>
+  <si>
+    <t>Product_Rating.csv: Table of Products with price and user ratings data</t>
+  </si>
+  <si>
+    <t>Index value for the anti-chafe product</t>
+  </si>
+  <si>
+    <t>Name of the product that it is being sold under</t>
+  </si>
+  <si>
+    <t>Distinguishing between different formulations; viscosity; etc. Creams are thinner like lotions; Ointments are thicker and most likely oil based; solids are very thick that are most likely applied from an applicator; liquids are sprayed or rolled on or rubbed in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some products are sold as "sport" products marketed specifically for sports use. General products are sold as anti-chafe but not for "sports" specifically. Off-Label products were identified in blogs; user forums; or from personal experience as good products ot use for sports; but not marketed as anti-chafe products for sports </t>
+  </si>
+  <si>
+    <t>If a product was marketed to "hikers" or "triathlon" of "bike" audiences this was captured. Bike products are meant for use in the "saddle" area applied to the groin and biking shorts padding or chamios.</t>
+  </si>
+  <si>
+    <t>Defines what area of the body this product is typically applied</t>
+  </si>
+  <si>
+    <t>Cost of the product (list price -- meaning that "discounts" or "specials" were ignored) in US dollars; 2016</t>
+  </si>
+  <si>
+    <t>Amount of the product in grams or mililiters. The density of water is 1g/ml. This may or may not be useful because of the nature of the product and how much is actually required in a typical application. One might put more "lotion" products on; but rub on a very small amount of a solid product.</t>
+  </si>
+  <si>
+    <t>Units of volume or mass: whether or not the product is mililiters or grams. Fluid Ounces was converted to mililiters for standardization</t>
+  </si>
+  <si>
     <t>Product_Unit_Cost</t>
-  </si>
-  <si>
-    <t>Reviews</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Rate_5</t>
-  </si>
-  <si>
-    <t>Rate_4</t>
-  </si>
-  <si>
-    <t>Rate_3</t>
-  </si>
-  <si>
-    <t>Rate_2</t>
-  </si>
-  <si>
-    <t>Rate_1</t>
-  </si>
-  <si>
-    <t>Product_Rating_Date</t>
-  </si>
-  <si>
-    <t>Rating_Source</t>
-  </si>
-  <si>
-    <t>Ingredient_Date</t>
-  </si>
-  <si>
-    <t>Ingredient_Source</t>
-  </si>
-  <si>
-    <t>Body Glide Origional</t>
-  </si>
-  <si>
-    <t>Solid</t>
-  </si>
-  <si>
-    <t>Sport</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Amazon.com</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Gold Bond Friction Defense</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Gold-Bond-Friction-Defense-Ounce/dp/B007VC9DKI</t>
-  </si>
-  <si>
-    <t>Skin Stong Slather</t>
-  </si>
-  <si>
-    <t>Cream</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>Brave Soldier Friction Zone</t>
-  </si>
-  <si>
-    <t>Ointment</t>
-  </si>
-  <si>
-    <t>Run; Bike</t>
-  </si>
-  <si>
-    <t>Trail Toes Foot and Body Cream</t>
-  </si>
-  <si>
-    <t>Run; Hike</t>
-  </si>
-  <si>
-    <t>Feet</t>
-  </si>
-  <si>
-    <t>HikeGoo Blister Prevention Cream (Feet)</t>
-  </si>
-  <si>
-    <t>Hike</t>
-  </si>
-  <si>
-    <t>rei.com</t>
-  </si>
-  <si>
-    <t>RunGoo Blister Prevention Cream</t>
-  </si>
-  <si>
-    <t>Rocket Pure Friction Therapy Natural Anti-Chafe Balm</t>
-  </si>
-  <si>
-    <t>Triathlon</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Anti-chafe-Protection-Triathletes-Ingredients-Rocket/dp/B00RKHRUFY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaseline </t>
-  </si>
-  <si>
-    <t>Chamois Butt'r</t>
-  </si>
-  <si>
-    <t>Bike</t>
-  </si>
-  <si>
-    <t>Groin</t>
-  </si>
-  <si>
-    <t>BikeBling.com</t>
-  </si>
-  <si>
-    <t>Blue Steel Sports Anti-Chafe Cream</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>Lanacane Anti-Chafing Gel</t>
-  </si>
-  <si>
-    <t>Gel</t>
-  </si>
-  <si>
-    <t>ChafeStop anti-chafing stick</t>
-  </si>
-  <si>
-    <t>2Toms SportShield Liquid Roll-On</t>
-  </si>
-  <si>
-    <t>Liquid</t>
-  </si>
-  <si>
-    <t>http://www.2toms.com/products-page/sportshield/sportshield-roll-on/</t>
-  </si>
-  <si>
-    <t>Mission Athletecare 5 Hour Anti-Chafe Cream</t>
-  </si>
-  <si>
-    <t>http://ec2-54-243-178-219.compute-1.amazonaws.com/skindeep/product/525433/MISSION_Athletecare_5_Hour_Anti-Chafe_Cream/</t>
-  </si>
-  <si>
-    <t>Trislide SBR Anti-Chafe Continuous Spray Lubricant</t>
-  </si>
-  <si>
-    <t>http://www.drugstore.com/trislide-aerosol-skin-lubricant/qxp277713</t>
-  </si>
-  <si>
-    <t>SLIK Anti-Friction and Anti-Chafe Skin Lube</t>
-  </si>
-  <si>
-    <t>http://skinstrong.com/slik-anti-chafing-spray/</t>
-  </si>
-  <si>
-    <t>Gooch Guard Chamois Cream</t>
-  </si>
-  <si>
-    <t>Zealios All Natural; Vegan; Betwixt Athletic Skin Lubricant and Chamois Cream</t>
-  </si>
-  <si>
-    <t>ChafeZone - Anti-Chafe and Blister Prevention</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/MedZone-ChafeZone-BurnZone-PainZone-LOT-of-20-NEW-First-Aid-Relief-Prevention-/151835007365</t>
-  </si>
-  <si>
-    <t>Mueller Lube Stick for Runners</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Mueller-Lube-Stick-Runners-2-25-Ounce/dp/B000TS8MHG/ref=pd_sim_sg_16</t>
-  </si>
-  <si>
-    <t>Corona Multi-Purpose Ointment</t>
-  </si>
-  <si>
-    <t>Off-Label</t>
-  </si>
-  <si>
-    <t>Veterinary</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Manna-Pro-0095005392-Purpose-Ointment/dp/B003ARD4TE/ref=sr_1_1?ie=UTF8&amp;qid=1456059201&amp;sr=8-1&amp;keywords=Corona+Multi-Purpose+Ointment</t>
-  </si>
-  <si>
-    <t>Boudreaux's Butt Paste Diaper Rash Ointment Skin Protectant</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Boudreauxs-Butt-Paste-Ointment-Protectant/dp/B001190D5Q/ref=sr_1_4?s=baby-products&amp;ie=UTF8&amp;qid=1456060126&amp;sr=1-4&amp;keywords=Butt+Paste</t>
-  </si>
-  <si>
-    <t>http://www.buttpaste.com/products/original-butt-paste</t>
-  </si>
-  <si>
-    <t>Sportslick</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Sportslick-3-8-oz/dp/B0007OC0A2/ref=sr_1_1?ie=UTF8&amp;qid=1456061443&amp;sr=8-1&amp;keywords=sportslick</t>
-  </si>
-  <si>
-    <t>http://www.allstarhealth.com/de_p/14001/Sportslick_The_Ultimate_Skin_Protector.htm</t>
-  </si>
-  <si>
-    <t>Ruby's Lube - All Natural Anti-Chafe Balm</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Rubys-Lube-Natural-Anti-Chafe-Balm/dp/B00MH7G8GO/ref=sr_1_15?ie=UTF8&amp;qid=1456078186</t>
-  </si>
-  <si>
-    <t>Bodyglide Skin Glide Anti-Friction Balm</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Bodyglide-Skin-Glide-Anti-Friction-Ounce/dp/B0031Y4S0U/ref=sr_1_2?ie=UTF8&amp;qid=1456079038</t>
-  </si>
-  <si>
-    <t>https://www.bodyglide.com/shop/skin/</t>
-  </si>
-  <si>
-    <t>Reflect Sports Hoo Ha Ride Glide</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Reflect-Sports-Ride-Glide-8-Ounce/dp/B009NN2O86</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/forum/-/Tx3RL6DD7J0OV22/ref=ask_dp_dpmw_al_hza?asin=B009NN2O86</t>
-  </si>
-  <si>
-    <t>Aquaphor (Baby)</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Aquaphor-Healing-Ointment-Diaper-Protectant/dp/B001F0RAVQ/ref=sr_1_5?ie=UTF8&amp;qid=1456089783</t>
-  </si>
-  <si>
-    <t>Surf Butta Anti-Chafe Balm</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Surf-Butta-Anti-Chafe-Balm-Eliminates/dp/B017HUPINY/ref=sr_1_9?s=sporting-goods&amp;ie=UTF8&amp;qid=1456090069</t>
-  </si>
-  <si>
-    <t>Chamois Butt'r GoStik Skin Lubricant</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Chamois-Buttr-GoStik-Lubricant-2-5-Ounce/dp/B00M8YXR74/ref=sr_1_18?s=sporting-goods&amp;ie=UTF8&amp;qid=1456090069</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Chamois-Buttr-GoStik-Lubricant-2-5-Ounce/dp/B00M8YXR74%3FSubscriptionId%3DAKIAJ7ULU7QZXKP7GIOQ%26tag%3Dhomea0c-20%26linkCode%3Dxm2%26camp%3D2025%26creative%3D165953%26creativeASIN%3DB00M8YXR74</t>
-  </si>
-  <si>
-    <t>Dead Down Wind Anti-Chafe + Anti-Itch Lotion</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Dead-Down-Wind-Anti-Chafe-Anti-Itch/dp/B00OH5LVLQ/ref=sr_1_1?ie=UTF8&amp;qid=1456091893</t>
-  </si>
-  <si>
-    <t>That Butt Stuff Anti Chafing Cream - Natural Chamois Balm</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Anti-Chafing-Cream-Natural-Chamois/dp/B002TIIGIO/ref=sr_1_31?s=sporting-goods&amp;ie=UTF8&amp;qid=1456107746</t>
-  </si>
-  <si>
-    <t>Petal Power Joy Ride Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/dp/B00PM94YC4?psc=1 PRICE information from manufactor website http://www.petal-power.com/store/p2/Petal_Power_Joy_Ride_Creme.html</t>
-  </si>
-  <si>
-    <t>http://www.petal-power.com/our-ingredients.html</t>
-  </si>
-  <si>
-    <t>DZ Nuts Pro Chamois Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/DZ-Nuts-Pro-Chamois-Cream/dp/B008F9J16M/ref=pd_sbs_468_5?ie=UTF8&amp;dpID=31ai7kgn6oL&amp;dpSrc=sims&amp;preST=_AC_UL160_SR160%2C160_&amp;refRID=1RF8866Y6MXDJFBDEJ84</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/forum/-/Tx4H8S2UKHM9D2/-/ref=ask_dp_lsw_al_hza?asin=B001C6DIF0  http://www.competitivecyclist.com/dz-nuts-pro-chamios-cream-mens</t>
-  </si>
-  <si>
-    <t>Soigneur Chamois Cream - Tempo</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Soigneur-Tempo-Chamois-Cream/dp/B009FPGHN0/ref=sr_1_1?ie=UTF8&amp;qid=1456200002</t>
-  </si>
-  <si>
-    <t>http://www.soigneur.net/shop/chamois-cream-1</t>
-  </si>
-  <si>
-    <t>Beach Gladiator Anti-Chafe Roll-On Rash Guard for Beach/Surf Rash</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Beach-Gladiator-Anti-Chafe-Roll--Guard/dp/B00RPOQMEC</t>
-  </si>
-  <si>
-    <t>Monistat Soothing Care Chafing Relief Powder-Gel</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Monistat-Soothing-Chafing-Powder-Gel-1-5-Ounce/dp/B0012ZNSWE</t>
-  </si>
-  <si>
-    <t>Assos Chamois Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Assos-Chamois-Cream-4-73-oz/dp/B001O19E2E</t>
-  </si>
-  <si>
-    <t>Udderly Smooth Chamois Cream with Shea Butter</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Udderly-Smooth-Chamois-Cream-Butter/dp/B00D86VJD0</t>
-  </si>
-  <si>
-    <t>Moraz Redskin - Polygonum Anti Chafe Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/dp/B001KYVWQG?psc=1</t>
-  </si>
-  <si>
-    <t>Bag-Balm; Vermonts Original Moisturizing and Softening Ointment</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Bag-Balm-Vermonts-Original-Moisturizing-Softening/dp/B0014CI4X8</t>
-  </si>
-  <si>
-    <t>Doc's Skin Care Chamois Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Docs-Skin-Care-Chamois-Cream/dp/B00EOUTNPA</t>
-  </si>
-  <si>
-    <t>http://docsskincare.com/products/chamois-cream/</t>
-  </si>
-  <si>
-    <t>Hammer Nutrition Seat Saver Chamois And Anti- Chafing Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Hammer-Nutrition-Saver-Chamois-Chafing/dp/B002K69HSI/</t>
-  </si>
-  <si>
-    <t>http://www.hammernutrition.com/products/seat-saver.ssv.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RunGuard Anti-Chafe Stick </t>
-  </si>
-  <si>
-    <t>https://www.google.com/shopping/product/4682990999738067527?q=RunGuard+Anti-Chafe&amp;biw=1192&amp;bih=578&amp;bav=on.2;or.r_cp.&amp;bvm=bv.115339255;d.dmo&amp;tch=1&amp;ech=1&amp;psi=pSzRVtiUAcHxeq6olYgH.1456549138121.9&amp;prds=hsec:reviews;paur:ClkAsKraX_JVZz_TOWlQw69jyl1NsFlF2fJED_TB-hXY0Ys4Ufb3VKbRAncj0n_e6kKDkYTBLlJNxS4V-4lKNaAn68oW1iNyTRR0HzndpgfJRZ2Ppr8O50f6xxIZAFPVH70i1tOHBnSoJG3SX9zlZEkaNSfmTQ&amp;ved=0ahUKEwjivqvilJfLAhVHGB4KHX1fB_AQqisIFQ&amp;ei=fC3RVuKQBseweP2-nYAP</t>
-  </si>
-  <si>
-    <t>http://www.runguards.com/products/runguard-original/ingredients</t>
-  </si>
-  <si>
-    <t>Fresh Balls</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Fresh-Balls-Oz-Tube-Pack/dp/B00D3LTEVE/#customerReviews</t>
-  </si>
-  <si>
-    <t>Akileïne Sports NOK Anti-chafing Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Akile%C3%AFne-Sports-Anti-chafing-Cream-75ml/dp/B0070X231Y; http://www.mec.ca/product/5009-478/sports-akileine-anti-friction-nok-cream-75ml/</t>
-  </si>
-  <si>
-    <t>http://www.cocooncenter.co.uk/akileine-sports-nok-anti-chafing-cream-75ml/8534.html#composition</t>
-  </si>
-  <si>
-    <t>Shea Butter Market SPLAX Anti‑Chafing Stick</t>
-  </si>
-  <si>
-    <t>http://www.mec.ca/product/5014-984/shea-butter-market-splax-anti-chafing-stick-60g/</t>
-  </si>
-  <si>
-    <t>http://www.artisancraftedbodycare.com/shea-butter-market-splax-anti-chafing-stick</t>
-  </si>
-  <si>
-    <t>Miracle of Aloe Chafe Guard Anti Friction Stick</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Miracle-Aloe-Lubricants-Eliminates-Comfortable/dp/B002FPBPOI</t>
-  </si>
-  <si>
-    <t>http://www.miracleofaloe.com/personal-care/problem-solvers/chafe-guard.html</t>
-  </si>
-  <si>
-    <t>Uberlube Luxury Lubricant</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Uberlube-UBER-100-Luxury-Lubricant-100ml/dp/B00502KJ2C</t>
-  </si>
-  <si>
-    <t>GurneyGoo Lubricant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General </t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/GurneyGears-GurneyGoo-Anti-Chafe-85ml/dp/B00SQ1DQY2</t>
-  </si>
-  <si>
-    <t>Desitin Maximum Strength Paste</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/dp/B003O32P8U/</t>
-  </si>
-  <si>
-    <t>https://www.desitin.com/diaper-rash-products/maximum-strength-original-zinc-oxide-paste</t>
-  </si>
-  <si>
-    <t>Hipoglos 4.2 Oz Baby Diaper Rash Cream And Skin Protectant</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Hipoglos-Baby-Diaper-Cream-Protectant/dp/B004DAQWAK</t>
-  </si>
-  <si>
-    <t>http://dailymed.nlm.nih.gov/dailymed/archives/fdaDrugInfo.cfm?archiveid=42792</t>
-  </si>
-  <si>
-    <t>Cramer Skin Lube</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Cramer-Legendary-Lubricant-Marathons-Triathlons/dp/B0002V8R70</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/NEW-Cramer-Skin-Lube-Pro-Strength-Lubricating-Ointment-1-Lb-Tub-192538-Chafing-/181714844162?hash=item2a4f0c7a02:g:lOMAAOSwNSxVKdu5</t>
-  </si>
-  <si>
-    <t>Waxelene Petroleum Jelly Alternative</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Waxelene-Petroleum-Jelly-Alternative-9-Ounce/dp/B00D3PMP20/</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/forum/-/Tx2LNYLMMZS5CUQ/-/ref=ask_dp_lsw_al_hza?asin=B00D3PMP20</t>
-  </si>
-  <si>
-    <t>Band-Aid Friction Blister Block Stick</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Band-Aid-Friction-Blister-Block-Stick/dp/B00166FZBG/</t>
-  </si>
-  <si>
-    <t>ChafeX Anti-Chafing Skin Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/gp/product/B00TT3KRMK/</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/forum/-/Tx2QO7ANIQVQO8C/ref=ask_dp_dpmw_al_hza?asin=B00TT3KRMK</t>
-  </si>
-  <si>
-    <t>Neat Feat 3B Body Saver Skin Chafing Antiperspirant Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Neat-Saver-Chafing-Antiperspirant-Ounces/dp/B00B5MPCWI</t>
-  </si>
-  <si>
-    <t>Neat 3B Action Cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.co.uk/dp/B001D8D7D0</t>
-  </si>
-  <si>
-    <t>3M Cavilon Durable Barrier Cream Fragrance Free</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/3M-Cavilon-Durable-Barrier-Fragrance/dp/B00CYPUUYK</t>
-  </si>
-  <si>
-    <t>http://solutions.3m.co.uk/wps/portal/3M/en_GB/Cavilon/skin-care/products/durable-barrier-cream/</t>
-  </si>
-  <si>
-    <t>Avon basics silicone glove hand cream</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/basics-silicone-glove-cream-3-4fl/dp/B0014HG8W2/</t>
-  </si>
-  <si>
-    <t>https://www.avon.com/product/41894/avon-care-silicone-glove-protective-hand-cream?setlang=en</t>
-  </si>
-  <si>
-    <t>Ingredient_Alternate_Name</t>
-  </si>
-  <si>
-    <t>Ingredient_Definition</t>
-  </si>
-  <si>
-    <t>Ingredient_Definition_Source</t>
-  </si>
-  <si>
-    <t>Ingredient_Def_Date</t>
-  </si>
-  <si>
-    <t>Ingredient_Chem_Ref</t>
-  </si>
-  <si>
-    <t>8-HYDROXYQUINOLINE</t>
-  </si>
-  <si>
-    <t>8-HYDROXYQUINOLINE is an antiseptic with mild fungistatic; bacteriostatic; anthelmintic; and amebicidal action. It is also used as a reagent and metal chelator; as a carrier for radio-indium for diagnostic purposes; and its halogenated derivatives are used in addition as topical anti-infective agents and oral antiamebics.</t>
-  </si>
-  <si>
-    <t>https://pubchem.ncbi.nlm.nih.gov/compound/8-hydroxyquinoline#section=Top</t>
-  </si>
-  <si>
-    <t>ACACIA DECURRENS Extract</t>
-  </si>
-  <si>
-    <t>About ACACIA DECURRENS FLOWER WAX: Acacia Decurrens Flower Wax is a wax obtained from the flowers of Acacia decurrens. Function(s): Skin-Conditioning Agent - Emollient; Skin-Conditioning Agent - Occlusive; SKIN CONDITIONING; SKIN PROTECTING</t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient/716261/ACACIA_DECURRENS_FLOWER_WAX/</t>
-  </si>
-  <si>
-    <t>Acai Juice</t>
-  </si>
-  <si>
-    <t>PH Control. Acetic Acid is an organic acid formed when ethanol is fermented. Vinegar is typically a 5% solution of Acetic Acid. Brown Rice Vinegar is the vinegar produced by the fermentation of unpolished brown rice. Natural Vinegars also contain small amounts of tartaric acid; citric acid and other acids. In cosmetics and personal care products; Acetic Acid; Vinegar and Brown Rice Vinegar are used in the formulation of hair conditioners; shampoos; hair rinses; wave sets and other hair care products. Acetic Acid is also used in mouthwashes and breath fresheners and Vinegar can be found in skin care products.</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/vinegar-and-acetic-acid</t>
-  </si>
-  <si>
-    <t>Acrylate Polymer</t>
-  </si>
-  <si>
-    <t>Binding agent. Acrylate polymer; "three" or "ter" in terpolymer means three monomers connected together.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Acrylate_polymer</t>
-  </si>
-  <si>
-    <t>Detatured Alcohol? Ethanol?</t>
-  </si>
-  <si>
-    <t>Unclear to which "alcohol" this is.</t>
-  </si>
-  <si>
-    <t>5-Ureidohydantoin; Glyoxyldiureide</t>
-  </si>
-  <si>
-    <t>llantoin is a naturally ocurring nitrogenous compound used as a skin conditioning agent.</t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient/700244/ALLANTOIN/</t>
-  </si>
-  <si>
-    <t>https://fscimage.fishersci.com/msds/24578.htm</t>
-  </si>
-  <si>
-    <t>Aloe Vera Extract; Aloe Vera Juice; Aloe Leaf Juice; Aloe Vera Gel</t>
-  </si>
-  <si>
-    <t>Juice vs. Gel -- Gel has a higher polysachride content; made from the inside of the plant. Juice is made from the outer leaf mainly. Gel has a higher concentration of aloin; which is a laxitive (why you should not drink the gel!)</t>
-  </si>
-  <si>
-    <t>http://www.livestrong.com/article/474409-aloe-vera-gel-vs-juice/ ; http://www.lilyofthedesert.com/faq/</t>
-  </si>
-  <si>
-    <t>Nutrients are transfered from the plant by mixing the gel with oil and sperating it out</t>
-  </si>
-  <si>
-    <t>http://www.aloeplant.info/how-to-make-aloe-vera-oil-for-skin/</t>
-  </si>
-  <si>
-    <t>ALUMINUM HYDROXYCHLORIDE</t>
-  </si>
-  <si>
-    <t>Aluminium chlorohydrate is a group of specific aluminium salts having the general formula AlnCl(3n-m)(OH)m. It is used in deodorants and antiperspirants and as a coagulant in water purification.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Aluminium_chlorohydrate</t>
-  </si>
-  <si>
-    <t>ALUMINUM SALT STARCH</t>
-  </si>
-  <si>
-    <t>This ingredient is an aluminum salt of chemically modified starch. Function(s): Absorbent; Anticaking Agent; Viscosity Increasing Agent - Nonaqueous; VISCOSITY CONTROLLING</t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient/700326/ALUMINUM_STARCH_OCTENYLSUCCINATE/</t>
-  </si>
-  <si>
-    <t>Prunus Armeniaca (Apricot) Oil; Bitter Almond Oil</t>
-  </si>
-  <si>
-    <t>Prunus Armeniaca (Apricot) Kernel Oil and Hydrogenated Apricot Oil function as skin conditioning agents - occlusive. Hydrogenated Apricot Kernel Oil also functions as a viscosity increasing agents - nonaqueous.</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/prunus-armeniaca-apricot-kernel-oil-and-hydrogenated-apricot-kernel-oil</t>
-  </si>
-  <si>
-    <t>ASCORBYL PALMITATE (VITAMIN C PALMITATE)</t>
-  </si>
-  <si>
-    <t>Ascorbyl palmitate is an ester formed from ascorbic acid and palmitic acid creating a fat-soluble form of vitamin C. In addition to its use as a source of vitamin C; it is also used as an antioxidant food additive (E number E304).</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Ascorbyl_palmitate</t>
-  </si>
-  <si>
-    <t>White Beeswax; Yellow Beeswax</t>
-  </si>
-  <si>
-    <t>Desyl Alcohol; Bitter Almond Oil Camphor</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Benzoin</t>
-  </si>
-  <si>
-    <t>BENZENEMETHANOL; BENZYLIC ALCOHOL; PHENYLCARBINOL; PHENYLMETHANOL; PHENYLMETHYL ALCOHOL;</t>
-  </si>
-  <si>
-    <t>External Analgesic; Fragrance Ingredient; Oral Health Care Drug; Preservative; Solvent;Viscosity Decreasing Agent; MASKING</t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient/700697/BENZYL_ALCOHOL/</t>
-  </si>
-  <si>
-    <t>http://chem.sis.nlm.nih.gov/chemidplus/name/benzyl%20alcohol</t>
-  </si>
-  <si>
-    <t>Beta-Carotene is a naturally occurring carotenoid pigment found in many fruits and vegetables. Beta-Carotene is a precursor of; and can be synthesized from; vitamin A. Beta-Carotene used in cosmetics and personal care products is prepared synthetically or obtained from natural sources.</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/beta-carotene</t>
-  </si>
-  <si>
-    <t>Butylated hydroxyanisole is an antioxidant consisting of a mixture of two isomeric organic compounds; 2-tert-butyl-4-hydroxyanisole and 3-tert-butyl-4-hydroxyanisole. It is prepared from 4-methoxyphenol and isobutylene</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Butylated_hydroxyanisole</t>
-  </si>
-  <si>
-    <t>Chamomile; Chamomile Extract</t>
-  </si>
-  <si>
-    <t>A resin obtained from Chamomile. Reduces sensitivity and inflammation.</t>
-  </si>
-  <si>
-    <t>https://www.dermalinstitute.com/us/library/glossary.html?l=B</t>
-  </si>
-  <si>
-    <t>Propellent</t>
-  </si>
-  <si>
-    <t>Butane is a gas commenly used as a propellent in aerosal sprays</t>
-  </si>
-  <si>
-    <t>Calendula officinalis Extract; Pot Marigold; Calendula Flower Extract; Calendula Flower Oil</t>
-  </si>
-  <si>
-    <t>In cosmetics and personal care products; Calendula Officinalis Extract; Calendula Officinalis Flower Extract and Calendula Officinalis Flower Oil function as skin conditioning agents - miscellaneous. Calendula Officinalis Flower Extract and Calendula Officinalis Flower Oil also function as fragrance ingredients. Calendula Officinalis Seed Oil functions as a skin conditioning agent - occlusive.</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/calendula-officinalis-derived-ingredients</t>
-  </si>
-  <si>
-    <t>These waxes also increase the thickness of the lipid (oil) portion of solid and stick-like products such as lipstick; giving them structure; allowing for a smooth application; and keeping them solid. Candelilla Wax is a yellowish-brown hard; brittle lustrous solid; extracted from the surface of the plant Euphorbia cerifera. In Europe this wax is known as Candelilla Cera.</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/beeswax-and-plant-waxes</t>
-  </si>
-  <si>
-    <t>Caprylic/Capric Triglycerides. * A mixed triester derived from coconut oil and glycerin. It comes in the form of an oily liquid; and is sometimes mistakenly referred to as fractionated coconut oil. Functions: Caprylic mainly works as an emollient; dispersing agent and solvent.</t>
-  </si>
-  <si>
-    <t>https://www.truthinaging.com/ingredients/capryliccapric-triglycerides</t>
-  </si>
-  <si>
-    <t>Properties: Effective humectant and emollient with antimicrobial efficacy; boosts traditional preservatives; provides deodorizing efficacy.</t>
-  </si>
-  <si>
-    <t>http://www.makingcosmetics.com/Caprylyl-Glycol-EHG_p_159.html</t>
-  </si>
-  <si>
-    <t>Castor Seed Oil; Ricinus Cummunis (Castor Seed) Oil</t>
-  </si>
-  <si>
-    <t>Ceresin wax</t>
-  </si>
-  <si>
-    <t>Cerin; Cerasin; Cerosin; Ceresin Wax; Ceresine</t>
-  </si>
-  <si>
-    <t>is a wax derived from ozokerite by a purifying process.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Ceresin</t>
-  </si>
-  <si>
-    <t>Cetearyl Alcohol and the other fatty alcohols keep an emulsion from separating into its oil and liquid components. These ingredients are also used to alter the thickness of liquid products and to increase foaming capacity or to stabilize foams.</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/cetearyl-alcohol-and-related-ingredients</t>
-  </si>
-  <si>
-    <t>Cetyl Esters NF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cetyl Esters Wax offers an easy way to increase the viscosity (thickness) of your creams and lotions while also improving the feel.  There is some confusion about the naturalness of this material because it is referred to as a synthetic Spermaceti Wax.  Spermaceti Wax is waxy liquid harvested from Whales; and when the industry realized that there was a demand for a more friendly approach they created the synthetic alternative; Cetyl Esters Wax; which is natural wax produced from coconut.  </t>
-  </si>
-  <si>
-    <t>http://www.ingredientstodiefor.com/item/Cetyl_Esters_NF/142/</t>
-  </si>
-  <si>
-    <t>Phenylacrylic acid</t>
-  </si>
-  <si>
-    <t>Cinnamic acid is an organic compound with the formula C6H5CHCHCO2H. It is a white crystalline compound that is slightly soluble in water; and freely soluble in many organic solvents. Classified as an unsaturated carboxylic acid; it occurs naturally in a number of plants.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Cinnamic_acid</t>
-  </si>
-  <si>
-    <t>Cocoa Seed Butter; Theobroma Cacao (Cocoa Seed) Butter</t>
-  </si>
-  <si>
-    <t>Comfrey; Comfrey Root Extract</t>
-  </si>
-  <si>
-    <t>CYCLOPENTASILOXANE</t>
-  </si>
-  <si>
-    <t>ANTISTATIC; EMOLLIENT; HAIR CONDITIONING; HUMECTANT; SOLVENT; VISCOSITY CONTROLLING</t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient/701738/CYCLOMETHICONE/</t>
-  </si>
-  <si>
-    <t>http://chem.sis.nlm.nih.gov/chemidplus/rn/69430-24-6</t>
-  </si>
-  <si>
-    <t>CYCLOPENTASILOXANE; DECAMETHYL-; DECAMETHYL- CYCLOPENTASILOXANE; DECAMETHYLCYCLOPENTASILOXANE</t>
-  </si>
-  <si>
-    <t>Decamethylcyclopentasiloxane is an organosilicon compound with the formula [(CH₃)₂SiO]₅. It is a colorless and odorless liquid that is slightly volatile. The compound is classified as a cyclomethicone.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Decamethylcyclopentasiloxane</t>
-  </si>
-  <si>
-    <t>https://pubchem.ncbi.nlm.nih.gov/compound/decamethylcyclopentasiloxane#section=Top</t>
-  </si>
-  <si>
-    <t>Methanol; Methyl Alcohol; Wood Alcohol</t>
-  </si>
-  <si>
-    <t>Diazolidnyl Urea</t>
-  </si>
-  <si>
-    <t>Diazolidinylurea</t>
-  </si>
-  <si>
-    <t>Diazolidinyl urea is an antimicrobial preservative used in cosmetics. It is chemically related to imidazolidinyl urea which is used in the same way. Diazolidinyl urea acts as a formaldehyde releaser.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Diazolidinyl_urea</t>
-  </si>
-  <si>
-    <t>http://www.commonchemistry.org/ChemicalDetail.aspx?ref=78491-02-8</t>
-  </si>
-  <si>
-    <t>Polydimethylsiloxane; Octamethyltrisiloxane; Dimethicone Crosspolymer</t>
-  </si>
-  <si>
-    <t>Polydimethylsiloxane belongs to a group of polymeric organosilicon compounds that are commonly referred to as silicones. PDMS is the most widely used silicon-based organic polymer; and is particularly known for its unusual rheological properties.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Polydimethylsiloxane</t>
-  </si>
-  <si>
-    <t>https://pubchem.ncbi.nlm.nih.gov/compound/24705</t>
-  </si>
-  <si>
-    <t>Ethylenediamine Tetraacetic Acid; Tetrasodium EDTA; Disodium EDTA</t>
-  </si>
-  <si>
-    <t>Disodium EDTA and the related ingredients bind to metal ions which inactivates them. The binding of metal ions helps prevent the deterioration of cosmetics and personal care products. It also helps to maintain clarity; protect fragrance compounds; and prevent rancidity.</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/edta-and-related-ingredients</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/ozokerite-and-other-fossil-and-synthetic-waxes</t>
-  </si>
-  <si>
-    <t>Ethylhexyglycerine</t>
-  </si>
-  <si>
-    <t>glycerine; propanetriol; 1;2;3-trihydroxypropane</t>
-  </si>
-  <si>
-    <t>Glycerol is a simple polyol (sugar alcohol) compound. It is a colorless; odorless; viscous liquid that is widely used in pharmaceutical formulations.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Glycerol</t>
-  </si>
-  <si>
-    <t>Glyceryl behenate is a fat used in cosmetics; foods; and oral pharmaceutical formulations. In cosmetics; it is mainly used as a viscosity-increasing agent in emulsions. Wikipedia</t>
-  </si>
-  <si>
-    <t>http://en.wikipedia.org/wiki/Glyceryl_behenate</t>
-  </si>
-  <si>
-    <t>https://pubchem.ncbi.nlm.nih.gov/compound/Glyceryl_behenate</t>
-  </si>
-  <si>
-    <t>Glycerin Stearate; Glycerol Monostearate</t>
-  </si>
-  <si>
-    <t>A humectant from the nectar of flowers.</t>
-  </si>
-  <si>
-    <t>https://www.dermalinstitute.com/us/library/glossary.html?l=H</t>
-  </si>
-  <si>
-    <t>Synthetic avenanthramide (Oat active)</t>
-  </si>
-  <si>
-    <t>Synthetic avenanthramide (Oat active) used to boost the efficacy of natural Oat.</t>
-  </si>
-  <si>
-    <t>Wax</t>
-  </si>
-  <si>
-    <t>Linalool is a naturally occurring fragrance substance produced by a wide variety of plants such as mint; cinnamon; citrus fruits; and birch trees. Linalool can also be produced synthetically.</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/linalool</t>
-  </si>
-  <si>
-    <t>Menthyl Lactate is a solid cooling agent and fragrance component for cosmetics. It is a derivative of Menthol; but is milder and more compatible with the skin.</t>
-  </si>
-  <si>
-    <t>http://www.makingcosmetics.com/Menthyl-Lactate_p_676.html</t>
-  </si>
-  <si>
-    <t>checkerberry oil; gaultheria oil; sweet birch oil; wintergreen oil</t>
-  </si>
-  <si>
-    <t>The methyl ester of salicylic acid; produced synthetically or distilled from Gaultheria procumbens (family Ericaceae) or from Betula lenta (family Betulaceae); used externally and internally for the treatment of various forms of rheumatism.</t>
-  </si>
-  <si>
-    <t>http://www.drugs.com/dict/methyl-salicylate.html</t>
-  </si>
-  <si>
-    <t>http://chem.sis.nlm.nih.gov/chemidplus/rn/119-36-8</t>
-  </si>
-  <si>
-    <t>Methylparaben is an anti-fungal agent often used in a variety of cosmetics and personal-care products. It is also used as a food preservative and has the E number E218.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Methylparaben</t>
-  </si>
-  <si>
-    <t>Paraffinum Liquidum; White Mineral Oil (Paraffinum Liquidum)</t>
-  </si>
-  <si>
-    <t>Octyldocecanol</t>
-  </si>
-  <si>
-    <t>Europaea (Olive) Fruit Unsaponifiables is a fraction of olive fruit remaining after fractional distillation.</t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient/721077/OLEA_EUROPAEA_%28OLIVE%29_FRUIT_UNSAPONIFIABLES/</t>
-  </si>
-  <si>
-    <t>Panthenol (pantothenol) is the alcohol analog of pantothenic acid (vitamin B5); and is thus a provitamin of B5. In organisms it is quickly oxidized to pantothenate [pantothenic acid]. In cosmetics and personal-care products; panthenol is a humectant; emollient; and moisturizer. In ointments; panthenol is an effective skin penetrator.[2] It is sometimes mixed with allantoin; in concentrations of up to 2-5%; and is used for treatment of sunburns; mild burns and minor skin disorders.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Panthenol</t>
-  </si>
-  <si>
-    <t>Myroxylon pereirae; Peruvian balsam; Indian balsam; black balsam; balsam Peru</t>
-  </si>
-  <si>
-    <t>Peru balsam is a tall tree that grows in Central America. This large tree often is cultivated as a shade tree. Crude Peru balsam is a dark brown; thick liquid with an aromatic smell of cinnamon and vanilla; and bitter taste. To remove it from the tree; the bark is alternately scorched and beaten.</t>
-  </si>
-  <si>
-    <t>http://www.drugs.com/npc/peru-balsam.html</t>
-  </si>
-  <si>
-    <t>Amur cork tree</t>
-  </si>
-  <si>
-    <t>Phellodendron amurense Rupr. is a species of tree in the family Rutaceae; commonly called the Amur cork tree. It is a major source of huáng bò (Chinese: 黄柏 or 黄檗); one of the 50 fundamental herbs used in traditional Chinese medicine. The Ainu people used this plant; called shikerebe-ni; as a painkiller</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Phellodendron_amurense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phenoxyethanol is an oily; slightly sticky liquid with a faint rose-like scent. It is used as a preservative in a wide variety of cosmetic and personal care products; including skin care products; eye makeup; fragrances; blushers; foundations; lipstick; bath soaps and detergents; etc. Research shows that this ingredient is safe when used in these products. </t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/phenoxyethanol</t>
-  </si>
-  <si>
-    <t>Polyphenylmethyl siloxane</t>
-  </si>
-  <si>
-    <t>Phenyl Trimethicone is a derivative of silica; or silcione; and is used in cosmetics and beauty products as an anti-foaming agent; hair conditioning agent; and skin-conditioning agent (Cosmetic Database)</t>
-  </si>
-  <si>
-    <t>https://www.truthinaging.com/ingredients/phenyl-trimethicone</t>
-  </si>
-  <si>
-    <t>https://pubchem.ncbi.nlm.nih.gov/compound/Phenyltris_trimethylsiloxy_silane#section=Top</t>
-  </si>
-  <si>
-    <t>Polygonum Aviculare</t>
-  </si>
-  <si>
-    <t>knotgrass; knotweed; pigweed</t>
-  </si>
-  <si>
-    <t>Polygonum aviculare or common knotgrass is a plant related to buckwheat and dock. It is also calledprostrate knotweed; birdweed; pigweed and lowgrass. It is an annual found in fields and wasteland; with white flowers from June to October. It is widespread across many countries in temperate regions; apparently native to Eurasia and North America; naturalized in temperate parts of the Southern Hemisphere.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Polygonum_aviculare</t>
-  </si>
-  <si>
-    <t>Gas used as a propellent in aerosol sprays</t>
-  </si>
-  <si>
-    <t>Propylene glycol; α-Propylene glycol; 1;2-Propanediol; 1;2-Dihydroxypropane; Methyl ethyl glycol (MEG); Methylethylene glycol</t>
-  </si>
-  <si>
-    <t>Propylene glycol; also called propane-1;2-diol; is an organic compound with the chemical formula C₃H₈O₂. It is a viscous colourless liquid which is nearly odourless but possesses a faintly sweet taste.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Propylene_glycol</t>
-  </si>
-  <si>
-    <t>Rosemary Leaf Extract; Rosmarinus Officinalis (Rosemary) Leaf Extract</t>
-  </si>
-  <si>
-    <t>beta hydroxy acid (abbreviated BHA);2-Hydroxybenzoic acid</t>
-  </si>
-  <si>
-    <t>Antiacne Agent; Antidandruff Agent; Corn/Callus/Wart Remover; Denaturant; Exfoliant;Fragrance Ingredient; Hair Conditioning Agent; Skin-Conditioning Agent - Miscellaneous; KERATOLYTIC; MASKING; PRESERVATIVE; SKIN CONDITIONING</t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient/705746/SALICYLIC_ACID/</t>
-  </si>
-  <si>
-    <t>http://chem.sis.nlm.nih.gov/chemidplus/name/salicylic%20acid</t>
-  </si>
-  <si>
-    <t>Silicone</t>
-  </si>
-  <si>
-    <t>2;4-hexadienoic acid</t>
-  </si>
-  <si>
-    <t>Sorbic acid (C6H8O2) is a natural preservative that comes from the rowan berries; Sorbus aucuparia (family Rosaceae). It is also prepared synthetically. It inhibits growth of fungi; yeast; mold and some bacteria and is nearly nontoxic to humans. Sorbic acid is safe to use in a wide range of foods; drugs; and cosmetic products. Sorbic acid and its salts; sodium sorbate; potassium sorbate and calcium sorbate are often used in food products as preservatives.</t>
-  </si>
-  <si>
-    <t>http://www.drugs.com/inactive/sorbic-acid-81.html</t>
-  </si>
-  <si>
-    <t>https://pubchem.ncbi.nlm.nih.gov/compound/643460</t>
-  </si>
-  <si>
-    <t>Soy Oil</t>
-  </si>
-  <si>
-    <t>Dimethicone; also known as polydimethylsiloxane; is a silicon-based polymer that is a man-made synthetic molecule made up of repeating units called monomers.  Silicon is the second most abundant element in the Earth's crust after oxygen; and silicon dioxide is also known as sand; commonly found on beaches and shores.  Dimethicone can also be found in many cooking oils; processed foods and in fast food items such as chicken nuggets and French fries</t>
-  </si>
-  <si>
-    <t>http://www.cosmeticsinfo.org/ingredient/stearyl-dimethicone</t>
-  </si>
-  <si>
-    <t>http://chem.sis.nlm.nih.gov/chemidplus/name/startswith/stearyl%20dimethicone</t>
-  </si>
-  <si>
-    <t>Steric Acid</t>
-  </si>
-  <si>
-    <t>Melaleuca Alternifolia (Tea Tree) Extract or Leaf Oil</t>
-  </si>
-  <si>
-    <t>Used for its antiseptic; analgesic and anti-bacterial properties; also aids in healing and soothing the skin.</t>
-  </si>
-  <si>
-    <t>https://www.dermalinstitute.com/us/library/glossary.html?l=M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triethanolamine is a strongly alkaline substance used as surfactant and pH adjusting chemical. Function(s): Fragrance Ingredient; pH Adjuster; Surfactant - Emulsifying Agent; BUFFERING; </t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient.php?ingred06=706639</t>
-  </si>
-  <si>
-    <t>OCTAMETHYL- TRISILOXANE; OCTAMETHYLTRISILOXANE; OCTAMETHYLTRISILOXANE; OCTAMETHYLTRISILOXANE; TRISILOXANE; OCTAMETHYL; TRISILOXANE; OCTAMETHYL-</t>
-  </si>
-  <si>
-    <t>About TRISILOXANE: Trisiloxane is a linear siloxane. Function(s): Antifoaming Agent; Skin-Conditioning Agent - Miscellaneous; SKIN CONDITIONING</t>
-  </si>
-  <si>
-    <t>http://www.ewg.org/skindeep/ingredient/706714/TRISILOXANE/</t>
-  </si>
-  <si>
-    <t>https://pubchem.ncbi.nlm.nih.gov/compound/vanillin#section=Top</t>
-  </si>
-  <si>
-    <t>Tocopheryl; Tocopherols; Tocopheryl Acetate Vitamin E Acetate; DL Alpha Tocopherol; Mixed Tocopherols</t>
-  </si>
-  <si>
-    <t>Tocopheryl acetate; also known as vitamin E acetate; is a common vitamin supplement with the molecular formula C31H52O3 (for 'α' form). It is the ester of acetic acid and tocopherol (vitamin E). It is often used indermatological products such as skin creams. Tocopheryl acetate is not oxidized and can penetrate through the skin to the living cells; where about 5% is converted to free tocopherol and provides beneficial antioxidant effects.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Tocopheryl_acetate</t>
-  </si>
-  <si>
-    <t>Aqua; Deionized Water</t>
-  </si>
-  <si>
-    <t>Epilobium Angustifolium; Willow Herb; Willow Herb Flower/Leaf/Stem Extract</t>
-  </si>
-  <si>
-    <t>Epilobium angustifolium is a PERENNIAL growing to 2 m (6ft) by 1 m (3ft 3in) at a fast rate.</t>
-  </si>
-  <si>
-    <t>http://www.pfaf.org/user/plant.aspx?LatinName=Epilobium+angustifolium</t>
-  </si>
-  <si>
-    <t>Achillea Millefolium</t>
-  </si>
-  <si>
-    <t>Achillea millefolium; commonly known as yarrow /ˈjæroʊ/ or common yarrow; is a flowering plant in the family Asteraceae. It is native to temperate regions of the Northern Hemisphere in Asia; Europe; and North America.[1] It has been introduced as a feed for live stock in places like New Zealand[2] and Australia. However; it is a weed in those places[2] and sometimes also in its native regions.[3]</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Achillea_millefolium</t>
-  </si>
-  <si>
-    <t>Zinc Oxide (CI 77947)</t>
-  </si>
-  <si>
-    <t>Zinc Stearate</t>
-  </si>
-  <si>
-    <t>General Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are no "blank" values; where no data was entered; the value of "na" was assigned. </t>
-  </si>
-  <si>
-    <t>Ingredients.csv: Assigns Ingredients to Products</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Index value for anti-chafe products from the Product_Rating table</t>
-  </si>
-  <si>
-    <t>Index value for anti-chafe ingredient from the Ingredient Defs (Definitions) table</t>
-  </si>
-  <si>
-    <t>Standardized ingredient name. Many products use different or alternate names. This provides some commonality.</t>
-  </si>
-  <si>
-    <t>Order of the ingredient from the product label. In theory; the first ingredient is the largest component; and listed in decending order</t>
-  </si>
-  <si>
-    <t>If a substitution was made for the common name; the original label ingredient listed is preserved here</t>
-  </si>
-  <si>
-    <t>Any minor notes about an ingredient for informational purposes</t>
-  </si>
-  <si>
-    <t>Product_Rating.csv: Table of Products with price and user ratings data</t>
-  </si>
-  <si>
-    <t>Index value for the anti-chafe product</t>
-  </si>
-  <si>
-    <t>Name of the product that it is being sold under</t>
-  </si>
-  <si>
-    <t>Distinguishing between different formulations; viscosity; etc. Creams are thinner like lotions; Ointments are thicker and most likely oil based; solids are very thick that are most likely applied from an applicator; liquids are sprayed or rolled on or rubbed in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some products are sold as "sport" products marketed specifically for sports use. General products are sold as anti-chafe but not for "sports" specifically. Off-Label products were identified in blogs; user forums; or from personal experience as good products ot use for sports; but not marketed as anti-chafe products for sports </t>
-  </si>
-  <si>
-    <t>If a product was marketed to "hikers" or "triathlon" of "bike" audiences this was captured. Bike products are meant for use in the "saddle" area applied to the groin and biking shorts padding or chamios.</t>
-  </si>
-  <si>
-    <t>Defines what area of the body this product is typically applied</t>
-  </si>
-  <si>
-    <t>Cost of the product (list price -- meaning that "discounts" or "specials" were ignored) in US dollars; 2016</t>
-  </si>
-  <si>
-    <t>Amount of the product in grams or mililiters. The density of water is 1g/ml. This may or may not be useful because of the nature of the product and how much is actually required in a typical application. One might put more "lotion" products on; but rub on a very small amount of a solid product.</t>
-  </si>
-  <si>
-    <t>Units of volume or mass: whether or not the product is mililiters or grams. Fluid Ounces was converted to mililiters for standardization</t>
   </si>
   <si>
     <t>Cost per gram or mililiter of product. This again may not be useful due to the amount of the product needed</t>
@@ -2960,7 +2963,7 @@
     <col customWidth="1" min="1" max="1" width="11.14"/>
     <col customWidth="1" min="2" max="2" width="15.0"/>
     <col customWidth="1" min="3" max="3" width="34.0"/>
-    <col customWidth="1" min="4" max="4" width="13.29"/>
+    <col customWidth="1" min="4" max="4" width="20.14"/>
     <col customWidth="1" min="5" max="5" width="46.86"/>
     <col customWidth="1" min="6" max="6" width="23.43"/>
   </cols>
@@ -19505,9 +19508,10 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="6.86"/>
     <col customWidth="1" min="2" max="2" width="54.86"/>
-    <col customWidth="1" min="3" max="3" width="11.0"/>
-    <col customWidth="1" min="4" max="4" width="10.71"/>
-    <col customWidth="1" min="5" max="6" width="9.0"/>
+    <col customWidth="1" min="3" max="3" width="12.57"/>
+    <col customWidth="1" min="4" max="4" width="18.57"/>
+    <col customWidth="1" min="5" max="5" width="24.57"/>
+    <col customWidth="1" min="6" max="6" width="9.0"/>
     <col customWidth="1" min="7" max="7" width="8.71"/>
     <col customWidth="1" min="8" max="8" width="8.57"/>
     <col customWidth="1" min="9" max="9" width="6.57"/>
@@ -37697,10 +37701,10 @@
     </row>
     <row r="24">
       <c r="A24" s="27" t="s">
-        <v>445</v>
+        <v>818</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="25">
@@ -37708,7 +37712,7 @@
         <v>446</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="26">
@@ -37716,7 +37720,7 @@
         <v>447</v>
       </c>
       <c r="B26" s="62" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="27">
@@ -37724,7 +37728,7 @@
         <v>448</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="28">
@@ -37732,7 +37736,7 @@
         <v>449</v>
       </c>
       <c r="B28" s="62" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="29">
@@ -37740,7 +37744,7 @@
         <v>450</v>
       </c>
       <c r="B29" s="62" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="30">
@@ -37748,7 +37752,7 @@
         <v>451</v>
       </c>
       <c r="B30" s="62" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="31">
@@ -37756,7 +37760,7 @@
         <v>452</v>
       </c>
       <c r="B31" s="62" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="32">
@@ -37764,7 +37768,7 @@
         <v>453</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="33">
@@ -37772,7 +37776,7 @@
         <v>454</v>
       </c>
       <c r="B33" s="62" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="34">
@@ -37780,7 +37784,7 @@
         <v>455</v>
       </c>
       <c r="B34" s="62" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="35">
@@ -37788,12 +37792,12 @@
         <v>456</v>
       </c>
       <c r="B35" s="62" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="60" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="38">
@@ -37809,7 +37813,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="62" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="40">
@@ -37825,7 +37829,7 @@
         <v>610</v>
       </c>
       <c r="B41" s="62" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="42">
@@ -37833,7 +37837,7 @@
         <v>611</v>
       </c>
       <c r="B42" s="62" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="43">
@@ -37841,7 +37845,7 @@
         <v>612</v>
       </c>
       <c r="B43" s="62" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="44">
@@ -37849,7 +37853,7 @@
         <v>613</v>
       </c>
       <c r="B44" s="62" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="45">
@@ -37857,7 +37861,7 @@
         <v>614</v>
       </c>
       <c r="B45" s="62" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>